<commit_message>
Holy hell, the model works
</commit_message>
<xml_diff>
--- a/SDVs/SDVs.xlsx
+++ b/SDVs/SDVs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\knech\OneDrive\Documents\ASE6002\ModelProject\SDVs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D9B213-4034-4D6E-92A4-C84144DC2C6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33C93A1-5026-4843-BC5D-FAAA704950F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{48F65717-2712-4319-979D-59E9A5CA4B1D}"/>
+    <workbookView xWindow="-37470" yWindow="465" windowWidth="25830" windowHeight="19215" xr2:uid="{48F65717-2712-4319-979D-59E9A5CA4B1D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -429,37 +429,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{470DD529-B9DA-4326-91F8-3E7A02BA4C7C}">
-  <dimension ref="B2:B6"/>
+  <dimension ref="B2:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>1</v>
       </c>
+      <c r="C2">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>2</v>
       </c>
+      <c r="C3">
+        <v>0.15</v>
+      </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>3</v>
       </c>
+      <c r="C4">
+        <v>0.4</v>
+      </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>0</v>
       </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>4</v>
+      </c>
+      <c r="C6">
+        <v>3000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>